<commit_message>
Se realizan cambios para sanity semilla 4
</commit_message>
<xml_diff>
--- a/build/resources/test/config_data/data.xlsx
+++ b/build/resources/test/config_data/data.xlsx
@@ -1,19 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sanity Ambientes\PrepaidAutomation\src\test\resources\config_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SanitySemilla4\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EE003E-B525-48E1-8CD2-021B9076B7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Semilla 4" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>MSIDN</t>
   </si>
@@ -111,15 +110,9 @@
     <t>3016875982</t>
   </si>
   <si>
-    <t>3016875893</t>
-  </si>
-  <si>
     <t>732111198172291</t>
   </si>
   <si>
-    <t>732111198172290</t>
-  </si>
-  <si>
     <t>Vendedor</t>
   </si>
   <si>
@@ -130,13 +123,52 @@
   </si>
   <si>
     <t>667299000</t>
+  </si>
+  <si>
+    <t>rutaWinWap</t>
+  </si>
+  <si>
+    <t>CQ10960370</t>
+  </si>
+  <si>
+    <t>Tigo.2022*</t>
+  </si>
+  <si>
+    <t>C:\Program Files (x86)\Winwap Technologies\WinWAP for Windows 4.2\WinWAP4.exe</t>
+  </si>
+  <si>
+    <t>984108505</t>
+  </si>
+  <si>
+    <t>835244140</t>
+  </si>
+  <si>
+    <t>3016877411</t>
+  </si>
+  <si>
+    <t>3016876876</t>
+  </si>
+  <si>
+    <t>732111198172293</t>
+  </si>
+  <si>
+    <t>732111198172294</t>
+  </si>
+  <si>
+    <t>311615530</t>
+  </si>
+  <si>
+    <t>3016877591</t>
+  </si>
+  <si>
+    <t>732111198172292</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +198,13 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF297BDE"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -188,7 +227,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -201,14 +240,9 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -523,24 +557,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="52.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="17.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="52.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -556,15 +590,24 @@
       <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -573,8 +616,17 @@
       <c r="E2" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -588,7 +640,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:8">
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
@@ -602,7 +654,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:8">
       <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
@@ -616,7 +668,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:8">
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
@@ -630,7 +682,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:8">
       <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
@@ -644,79 +696,99 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="6"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="B9" s="7"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="8" t="s">
+    <row r="8" spans="1:8">
+      <c r="A8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>34</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega nuevo caso de uso para sanity semilla 4, CambioPosPre
</commit_message>
<xml_diff>
--- a/build/resources/test/config_data/data.xlsx
+++ b/build/resources/test/config_data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Semilla 4" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="58">
   <si>
     <t>MSIDN</t>
   </si>
@@ -51,139 +51,154 @@
     <t>http://10.69.60.85:8280/portal/login?initialURI=%2Fportal%2FCRMPortal</t>
   </si>
   <si>
+    <t>http://10.65.45.12:9001/gatewaycbs/BcServicesInt</t>
+  </si>
+  <si>
+    <t>URL DB</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>10.69.60.89</t>
+  </si>
+  <si>
+    <t>DEV11G</t>
+  </si>
+  <si>
+    <t>ACTIVATOR</t>
+  </si>
+  <si>
+    <t>10.69.60.88</t>
+  </si>
+  <si>
+    <t>desepos</t>
+  </si>
+  <si>
+    <t>epos</t>
+  </si>
+  <si>
+    <t>dev10g</t>
+  </si>
+  <si>
+    <t>postsale</t>
+  </si>
+  <si>
+    <t>10.65.32.74</t>
+  </si>
+  <si>
+    <t>siebel04</t>
+  </si>
+  <si>
+    <t>siebel</t>
+  </si>
+  <si>
+    <t>service</t>
+  </si>
+  <si>
+    <t>http://10.65.45.12:9001/gatewaymgint/GatewayMGWSInt</t>
+  </si>
+  <si>
+    <t>MSI</t>
+  </si>
+  <si>
+    <t>3016875982</t>
+  </si>
+  <si>
+    <t>732111198172291</t>
+  </si>
+  <si>
+    <t>Vendedor</t>
+  </si>
+  <si>
+    <t>Cedula Cliente</t>
+  </si>
+  <si>
+    <t>10960370</t>
+  </si>
+  <si>
+    <t>667299000</t>
+  </si>
+  <si>
+    <t>rutaWinWap</t>
+  </si>
+  <si>
+    <t>CQ10960370</t>
+  </si>
+  <si>
+    <t>Tigo.2022*</t>
+  </si>
+  <si>
+    <t>C:\Program Files (x86)\Winwap Technologies\WinWAP for Windows 4.2\WinWAP4.exe</t>
+  </si>
+  <si>
+    <t>984108505</t>
+  </si>
+  <si>
+    <t>835244140</t>
+  </si>
+  <si>
+    <t>3016877411</t>
+  </si>
+  <si>
+    <t>3016876876</t>
+  </si>
+  <si>
+    <t>732111198172293</t>
+  </si>
+  <si>
+    <t>732111198172294</t>
+  </si>
+  <si>
+    <t>311615530</t>
+  </si>
+  <si>
+    <t>3016877591</t>
+  </si>
+  <si>
+    <t>732111198172292</t>
+  </si>
+  <si>
+    <t>http://10.69.60.106:8180/tigo-pos-web/wap/windex.wml</t>
+  </si>
+  <si>
+    <t>http://10.69.60.107:8080/CRMPortal/auth/portal/default/Venta</t>
+  </si>
+  <si>
+    <t>http://10.69.60.106:8180/tigo-pos-web/index.jsp</t>
+  </si>
+  <si>
+    <t>10.69.60.103</t>
+  </si>
+  <si>
+    <t>10.69.60.102</t>
+  </si>
+  <si>
+    <t>10.65.32.76</t>
+  </si>
+  <si>
+    <t>SIEBEL02</t>
+  </si>
+  <si>
+    <t>874513783</t>
+  </si>
+  <si>
+    <t>680974538</t>
+  </si>
+  <si>
+    <t>1016141153</t>
+  </si>
+  <si>
+    <t>499757452</t>
+  </si>
+  <si>
+    <t>624917673</t>
+  </si>
+  <si>
     <t>http://10.69.60.77:8180/tigo-pos-web/wap/windex.wml</t>
-  </si>
-  <si>
-    <t>http://10.65.45.12:9001/gatewaycbs/BcServicesInt</t>
-  </si>
-  <si>
-    <t>URL DB</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>10.69.60.89</t>
-  </si>
-  <si>
-    <t>DEV11G</t>
-  </si>
-  <si>
-    <t>ACTIVATOR</t>
-  </si>
-  <si>
-    <t>10.69.60.88</t>
-  </si>
-  <si>
-    <t>desepos</t>
-  </si>
-  <si>
-    <t>epos</t>
-  </si>
-  <si>
-    <t>dev10g</t>
-  </si>
-  <si>
-    <t>postsale</t>
-  </si>
-  <si>
-    <t>10.65.32.74</t>
-  </si>
-  <si>
-    <t>siebel04</t>
-  </si>
-  <si>
-    <t>siebel</t>
-  </si>
-  <si>
-    <t>service</t>
-  </si>
-  <si>
-    <t>http://10.65.45.12:9001/gatewaymgint/GatewayMGWSInt</t>
-  </si>
-  <si>
-    <t>MSI</t>
-  </si>
-  <si>
-    <t>3016875982</t>
-  </si>
-  <si>
-    <t>732111198172291</t>
-  </si>
-  <si>
-    <t>Vendedor</t>
-  </si>
-  <si>
-    <t>Cedula Cliente</t>
-  </si>
-  <si>
-    <t>10960370</t>
-  </si>
-  <si>
-    <t>667299000</t>
-  </si>
-  <si>
-    <t>rutaWinWap</t>
-  </si>
-  <si>
-    <t>CQ10960370</t>
-  </si>
-  <si>
-    <t>Tigo.2022*</t>
-  </si>
-  <si>
-    <t>C:\Program Files (x86)\Winwap Technologies\WinWAP for Windows 4.2\WinWAP4.exe</t>
-  </si>
-  <si>
-    <t>984108505</t>
-  </si>
-  <si>
-    <t>835244140</t>
-  </si>
-  <si>
-    <t>3016877411</t>
-  </si>
-  <si>
-    <t>3016876876</t>
-  </si>
-  <si>
-    <t>732111198172293</t>
-  </si>
-  <si>
-    <t>732111198172294</t>
-  </si>
-  <si>
-    <t>311615530</t>
-  </si>
-  <si>
-    <t>3016877591</t>
-  </si>
-  <si>
-    <t>732111198172292</t>
-  </si>
-  <si>
-    <t>http://10.69.60.106:8180/tigo-pos-web/wap/windex.wml</t>
-  </si>
-  <si>
-    <t>http://10.69.60.107:8080/CRMPortal/auth/portal/default/Venta</t>
-  </si>
-  <si>
-    <t>http://10.69.60.106:8180/tigo-pos-web/index.jsp</t>
-  </si>
-  <si>
-    <t>10.69.60.103</t>
-  </si>
-  <si>
-    <t>10.69.60.102</t>
-  </si>
-  <si>
-    <t>10.65.32.76</t>
-  </si>
-  <si>
-    <t>SIEBEL02</t>
   </si>
 </sst>
 </file>
@@ -582,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
@@ -613,13 +628,13 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="H1" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -630,176 +645,176 @@
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="D4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="D5" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="D6" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -819,7 +834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -849,193 +864,193 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="H1" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1">
       <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1">
       <c r="A4" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="D4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1">
       <c r="A5" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="D5" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="D6" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1">
       <c r="A7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="C7" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1">
       <c r="A8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="1" customFormat="1">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="1" customFormat="1">
       <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="C11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="1" customFormat="1">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="1" customFormat="1">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>